<commit_message>
Fixed a bug in IvtffText and improved concordance version.
</commit_message>
<xml_diff>
--- a/resources/analysis/MostUsedTerms.xlsx
+++ b/resources/analysis/MostUsedTerms.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mzatt\Projects\Git - v4j\resources\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DA4D89-E6A3-467B-BBB2-08ABDBEB3994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83BE513-F7D6-428D-8D44-46D477FC1CB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7785" yWindow="180" windowWidth="17625" windowHeight="15015" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7785" yWindow="180" windowWidth="17625" windowHeight="15015" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="2" r:id="rId1"/>
     <sheet name="Analysis" sheetId="3" r:id="rId2"/>
-    <sheet name="Terms only in one cluster" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Terms only in one cluster" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Analysis!$A$1:$G$65</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Raw Data'!$A$4:$E$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$G$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="79">
   <si>
     <t>Cluster</t>
   </si>
@@ -271,6 +273,9 @@
   </si>
   <si>
     <t>Do not use this for filtering as the lookup formula will mess up</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -3021,9 +3026,9 @@
   </sheetPr>
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L33" sqref="L33"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="A1:G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5047,11 +5052,1528 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B668CEA-E766-4D50-B577-4C116C6A0148}">
+  <dimension ref="A1:G65"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1.27413127413127E-2</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2.0666255397902501E-2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1.8730779983226101E-2</v>
+      </c>
+      <c r="G2" s="9">
+        <v>2.0750988142292402E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="9">
+        <v>5.9288537549407102E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1.27667505358307E-2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1.9762845849802299E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="9">
+        <v>4.9407114624505904E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1.4188772362739001E-2</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1.3698630136986301E-2</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1.6798418972331999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1.0795805058605799E-2</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1.6347933374460201E-2</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1.9740900678593399E-2</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3.1079919793755299E-2</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1.7985276302301699E-2</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="9">
+        <v>6.9890970086664804E-3</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1.42857142857142E-2</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="9">
+        <v>8.8803088803088796E-3</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="9">
+        <v>4.9407114624505904E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="9">
+        <v>6.2815785880103699E-3</v>
+      </c>
+      <c r="C13" s="9">
+        <v>8.8803088803088796E-3</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1.34631910627327E-2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1.16484950144441E-2</v>
+      </c>
+      <c r="G13" s="9">
+        <v>5.9288537549407102E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="9">
+        <v>2.7174655195957902E-2</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1.77606177606177E-2</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="9">
+        <v>6.2435933277420501E-3</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1.8708179707770001E-2</v>
+      </c>
+      <c r="C15" s="9">
+        <v>8.8803088803088796E-3</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1.21534890072374E-2</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="9">
+        <v>6.5546907005325601E-3</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="9">
+        <v>5.5987983067048996E-3</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1.33824935135873E-2</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="9">
+        <v>5.1618189266693898E-2</v>
+      </c>
+      <c r="C20" s="9">
+        <v>4.0926640926640903E-2</v>
+      </c>
+      <c r="D20" s="10">
+        <v>2.3442319555829701E-2</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1.2603838441707199E-2</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1.4350945857795099E-2</v>
+      </c>
+      <c r="G20" s="9">
+        <v>7.9051383399209394E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="9">
+        <v>9.6954799945377507E-3</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1.27413127413127E-2</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1.01690060154683E-2</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="9">
+        <v>9.1492557694933703E-3</v>
+      </c>
+      <c r="C23" s="9">
+        <v>8.8803088803088796E-3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1.5114127082048101E-2</v>
+      </c>
+      <c r="E23" s="9">
+        <v>1.04554568891435E-2</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="9">
+        <v>5.9288537549407102E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="9">
+        <v>5.7353543629659904E-3</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="9">
+        <v>1.37921616823706E-2</v>
+      </c>
+      <c r="C25" s="9">
+        <v>7.3359073359073297E-3</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1.11042566317088E-2</v>
+      </c>
+      <c r="E25" s="9">
+        <v>7.8773990260670203E-3</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="9">
+        <v>5.9288537549407102E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="9">
+        <v>8.3070753365797698E-3</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="9">
+        <v>6.91699604743083E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1.04873534855027E-2</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="9">
+        <v>1.0530239493057401E-2</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="10">
+        <v>7.7112893275755696E-3</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="9">
+        <v>6.91699604743083E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="10">
+        <v>9.8704503392967307E-3</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="10">
+        <v>7.7112893275755696E-3</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="9">
+        <v>9.6525096525096506E-3</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="9">
+        <v>8.6664802907464294E-3</v>
+      </c>
+      <c r="G32" s="9">
+        <v>4.9407114624505904E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1.0424710424710401E-2</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="9">
+        <v>7.3359073359073297E-3</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="9">
+        <v>7.5105830943602301E-3</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1.38996138996138E-2</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1.01789019123997E-2</v>
+      </c>
+      <c r="E35" s="9">
+        <v>3.4803781151532501E-2</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1.0064299692479701E-2</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="9">
+        <v>7.6471391506213304E-3</v>
+      </c>
+      <c r="C36" s="9">
+        <v>1.27413127413127E-2</v>
+      </c>
+      <c r="D36" s="10">
+        <v>2.0666255397902501E-2</v>
+      </c>
+      <c r="E36" s="9">
+        <v>9.7393297049556005E-3</v>
+      </c>
+      <c r="F36" s="9">
+        <v>5.9640294473953899E-3</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="9">
+        <v>8.2937284502842198E-3</v>
+      </c>
+      <c r="G37" s="9">
+        <v>6.91699604743083E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="10">
+        <v>6.16903146206045E-3</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="10">
+        <v>6.7859346082665001E-3</v>
+      </c>
+      <c r="E39" s="9">
+        <v>7.73417358922944E-3</v>
+      </c>
+      <c r="F39" s="9">
+        <v>5.6844655670487297E-3</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G40" s="9">
+        <v>1.0869565217391301E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G41" s="9">
+        <v>8.8932806324110592E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G42" s="9">
+        <v>5.9288537549407102E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G43" s="9">
+        <v>4.9407114624505904E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G44" s="9">
+        <v>4.9407114624505904E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="10">
+        <v>6.16903146206045E-3</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1.36064164995703E-2</v>
+      </c>
+      <c r="F45" s="9">
+        <v>1.45373217780262E-2</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="9">
+        <v>2.1913491836150101E-2</v>
+      </c>
+      <c r="F46" s="9">
+        <v>5.6844655670487297E-3</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1.6184474362646799E-2</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="10">
+        <v>8.6366440468846391E-3</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="10">
+        <v>1.2029611351017801E-2</v>
+      </c>
+      <c r="E49" s="9">
+        <v>2.33457462045259E-2</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="9">
+        <v>2.23431681466628E-2</v>
+      </c>
+      <c r="F50" s="9">
+        <v>1.2673562575715201E-2</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" s="9">
+        <v>7.7220077220077196E-3</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="9">
+        <v>1.2603838441707199E-2</v>
+      </c>
+      <c r="F51" s="9">
+        <v>1.48168856583729E-2</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="9">
+        <v>8.8803088803088796E-3</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="9">
+        <v>7.7220077220077196E-3</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="9">
+        <v>8.7367516470925194E-3</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="9">
+        <v>1.73302778573474E-2</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" s="9">
+        <v>6.2815785880103699E-3</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="9">
+        <v>1.6659838863853599E-2</v>
+      </c>
+      <c r="C57" s="9">
+        <v>1.0424710424710401E-2</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" s="10">
+        <v>1.11042566317088E-2</v>
+      </c>
+      <c r="E58" s="9">
+        <v>3.6092810083070699E-2</v>
+      </c>
+      <c r="F58" s="9">
+        <v>1.09961792936352E-2</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="9">
+        <v>7.3359073359073297E-3</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" s="9">
+        <v>1.41793182469206E-2</v>
+      </c>
+      <c r="F59" s="9">
+        <v>8.0141645699375597E-3</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="9">
+        <v>1.09244845008876E-2</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="9">
+        <v>1.25631571760207E-2</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" s="9">
+        <v>7.9202512631435205E-3</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" s="9">
+        <v>7.1009149255769396E-3</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G64" s="9">
+        <v>6.91699604743083E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="11">
+        <v>0.25645227365833634</v>
+      </c>
+      <c r="C65" s="11">
+        <v>0.23745173745173703</v>
+      </c>
+      <c r="D65" s="12">
+        <v>0.24892041949413884</v>
+      </c>
+      <c r="E65" s="11">
+        <v>0.33256946433686568</v>
+      </c>
+      <c r="F65" s="11">
+        <v>0.2183393905507402</v>
+      </c>
+      <c r="G65" s="11">
+        <v>0.16699604743082982</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G65" xr:uid="{6DF483A8-CDFA-445A-9667-3A935CCE26BE}"/>
+  <conditionalFormatting sqref="B2:G64">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242C21BC-8281-464E-A29E-5A0A39530012}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>